<commit_message>
Added Family Number attribute
</commit_message>
<xml_diff>
--- a/data/occupation_classes_new.xlsx
+++ b/data/occupation_classes_new.xlsx
@@ -2273,9 +2273,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C476"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A246" sqref="A246:C246"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="43.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>